<commit_message>
add tasks for Log4j,JUnit,Hibernate,Wiki updates
</commit_message>
<xml_diff>
--- a/Dave Sullivan Individual Project Plan.xlsx
+++ b/Dave Sullivan Individual Project Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\Education\Enterprise Java\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dave\Documents\GitHub\Project-Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Dave Sullivan -Enterprise Java, Individaul Project Plan</t>
   </si>
@@ -60,6 +60,18 @@
   </si>
   <si>
     <t>Research the permutations logic to establish combinations business logic.</t>
+  </si>
+  <si>
+    <t>Wiki update</t>
+  </si>
+  <si>
+    <t>Log4j</t>
+  </si>
+  <si>
+    <t>Junit tests</t>
+  </si>
+  <si>
+    <t>Hibernate</t>
   </si>
 </sst>
 </file>
@@ -399,32 +411,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -432,7 +460,7 @@
         <v>42275</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -440,7 +468,7 @@
         <v>42282</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -448,7 +476,7 @@
         <v>42296</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -456,7 +484,7 @@
         <v>42303</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -464,7 +492,7 @@
         <v>42310</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -472,7 +500,7 @@
         <v>42324</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -480,7 +508,7 @@
         <v>42338</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>7</v>
       </c>

</xml_diff>